<commit_message>
input year into boundary
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8349BF3F-BABC-4693-BCB3-1379F69352F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EFC634-18F6-4BCA-9A9A-7D3431775A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>LO</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -323,10 +326,10 @@
   <cellStyles count="7">
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
     <cellStyle name="Neutral 3" xfId="3" xr:uid="{5B3B309E-6B7E-4D77-AD41-EB17FF9CE808}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{A93E1CA5-B318-4E00-82A5-334EC04E563E}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{C11532E7-AD97-42AD-83FD-AF150A506CCF}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="1" xr:uid="{5884504C-975A-4531-8909-E98FC51AE458}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="4" xr:uid="{8D4A26F5-E00A-421E-B82B-A50A6798403B}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,57 +608,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:P12"/>
+  <dimension ref="C2:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.265625" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -663,14 +669,15 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -678,41 +685,44 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="14"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="14"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -724,80 +734,90 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-    </row>
-    <row r="10" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="H10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="I10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="J10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="K10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="L10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="M10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="N10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="18"/>
       <c r="O10" s="18"/>
       <c r="P10" s="18"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="D11" t="s">
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2030</v>
+      </c>
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1000</v>
       </c>
-      <c r="I11" s="19">
+      <c r="J11" s="19">
         <v>1000</v>
       </c>
-      <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-      <c r="L11" t="s">
+      <c r="L11" s="19"/>
+      <c r="M11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="D12" t="s">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2030</v>
+      </c>
+      <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1000</v>
       </c>
-      <c r="I12" s="19">
+      <c r="J12" s="19">
         <v>1000</v>
       </c>
-      <c r="J12" s="19"/>
       <c r="K12" s="19"/>
-      <c r="L12" t="s">
+      <c r="L12" s="19"/>
+      <c r="M12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
input cable activity lower bound
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EFC634-18F6-4BCA-9A9A-7D3431775A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35487822-6BAB-431F-ACC0-1958CF7CB6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -76,6 +85,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKE_DKISLBH_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKW_DKISL1_01</t>
+  </si>
+  <si>
+    <t>ACT_BND</t>
   </si>
 </sst>
 </file>
@@ -608,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:Q12"/>
+  <dimension ref="C2:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,6 +839,100 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+    </row>
+    <row r="16" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>2030</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="M17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>2030</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update lower activity cable boundary
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35487822-6BAB-431F-ACC0-1958CF7CB6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584792D-918A-457C-BAC4-F650F076C384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="C2:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +909,9 @@
       <c r="F17" t="s">
         <v>19</v>
       </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
       <c r="I17">
         <v>10</v>
       </c>
@@ -925,6 +928,9 @@
       </c>
       <c r="F18" t="s">
         <v>19</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
       </c>
       <c r="J18">
         <v>10</v>

</xml_diff>

<commit_message>
change in boundaries towards the planned capacities
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584792D-918A-457C-BAC4-F650F076C384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C50A0B-9664-4774-8B7F-84850FE5A103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16008" yWindow="1212" windowWidth="21012" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -629,17 +629,17 @@
   <dimension ref="C2:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -651,7 +651,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -663,7 +663,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -679,7 +679,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -695,7 +695,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -711,7 +711,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -723,7 +723,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -735,7 +735,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
         <v>8</v>
       </c>
@@ -795,7 +795,7 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>2030</v>
       </c>
@@ -806,10 +806,10 @@
         <v>13</v>
       </c>
       <c r="I11">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J11" s="19">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
@@ -817,7 +817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D12">
         <v>2030</v>
       </c>
@@ -828,10 +828,10 @@
         <v>13</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J12" s="19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
@@ -839,10 +839,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="15" t="s">
-        <v>7</v>
-      </c>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>2045</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>3000</v>
+      </c>
+      <c r="J13">
+        <v>3500</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>2045</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>3500</v>
+      </c>
+      <c r="M14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
@@ -858,7 +896,7 @@
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
@@ -899,7 +937,7 @@
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>2030</v>
       </c>
@@ -919,7 +957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>2030</v>
       </c>

</xml_diff>

<commit_message>
Change H2 Export lower boundary
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA98ABD6-9C53-4C4A-9E87-814E9CF8AAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2432CCA-F75F-4DBB-AA2E-88D39B76B3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="5325" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,23 +162,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="60"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -198,7 +181,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,24 +191,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -241,20 +206,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -269,21 +225,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -292,9 +233,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -308,29 +249,8 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -338,11 +258,12 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
@@ -629,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:Q25"/>
+  <dimension ref="C2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
@@ -640,303 +561,282 @@
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="23.28515625" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="17" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D11">
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12">
         <v>2030</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I11">
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12">
         <v>2000</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="13">
         <v>3000</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" t="s">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D12">
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12">
         <v>2030</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I12">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12">
         <v>0</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="13">
         <v>0</v>
       </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" t="s">
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D13">
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12">
         <v>2045</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I13">
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12">
         <v>3000</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="12">
         <v>3500</v>
       </c>
-      <c r="M13" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D14">
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12">
         <v>2045</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I14">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12">
         <v>0</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="12">
         <v>3500</v>
       </c>
-      <c r="M14" t="s">
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="15" t="s">
+      <c r="N14" s="12"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-    </row>
-    <row r="17" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="17" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L17" s="18" t="s">
+      <c r="L17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+    </row>
+    <row r="18" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>2030</v>
       </c>
@@ -947,16 +847,52 @@
         <v>19</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="V18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="W18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:31" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>2045</v>
       </c>
@@ -967,95 +903,38 @@
         <v>19</v>
       </c>
       <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19">
+        <v>2030</v>
+      </c>
+      <c r="V19" t="s">
         <v>15</v>
       </c>
-      <c r="M19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-    </row>
-    <row r="23" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="L23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-    </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D24">
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="U20">
         <v>2030</v>
       </c>
-      <c r="E24" t="s">
+      <c r="V20" t="s">
         <v>15</v>
       </c>
-      <c r="F24" t="s">
+      <c r="W20" t="s">
         <v>19</v>
       </c>
-      <c r="M24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D25">
-        <v>2030</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="AD20" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding a seperate file to control the H2 Export Demand
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2432CCA-F75F-4DBB-AA2E-88D39B76B3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F970E5BA-689D-45F4-82F6-83EF30688432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>ACT_BND</t>
-  </si>
-  <si>
-    <t>EXPH2*</t>
   </si>
 </sst>
 </file>
@@ -552,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,9 +768,7 @@
       <c r="N14" s="12"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
@@ -786,43 +781,7 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>10</v>
-      </c>
+    <row r="17" spans="10:31" x14ac:dyDescent="0.25">
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -836,25 +795,11 @@
       <c r="AD17" s="9"/>
       <c r="AE17" s="9"/>
     </row>
-    <row r="18" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18">
-        <v>2030</v>
-      </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="10:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="M18" s="12"/>
       <c r="T18" s="10" t="s">
         <v>8</v>
       </c>
@@ -892,25 +837,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="D19">
-        <v>2045</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
+    <row r="19" spans="10:31" x14ac:dyDescent="0.25">
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
-      <c r="M19" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="M19" s="12"/>
       <c r="U19">
         <v>2030</v>
       </c>
@@ -924,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:31" x14ac:dyDescent="0.25">
       <c r="U20">
         <v>2030</v>
       </c>

</xml_diff>

<commit_message>
force to build ammonia capacity
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F970E5BA-689D-45F4-82F6-83EF30688432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC140493-8719-4AA5-A73B-0AE20B3472D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>ACT_BND</t>
+  </si>
+  <si>
+    <t>SUPELCAMM01</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -222,8 +225,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -231,8 +243,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -261,13 +274,15 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="7" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
     <cellStyle name="Neutral 3" xfId="3" xr:uid="{5B3B309E-6B7E-4D77-AD41-EB17FF9CE808}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{A93E1CA5-B318-4E00-82A5-334EC04E563E}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{C11532E7-AD97-42AD-83FD-AF150A506CCF}"/>
+    <cellStyle name="Normal 42" xfId="7" xr:uid="{5C9F8D4D-0E13-4029-9DD1-AB51B39E1F9C}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="1" xr:uid="{5884504C-975A-4531-8909-E98FC51AE458}"/>
     <cellStyle name="Standard 2" xfId="4" xr:uid="{8D4A26F5-E00A-421E-B82B-A50A6798403B}"/>
   </cellStyles>
@@ -550,7 +565,7 @@
   <dimension ref="C2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="N19" sqref="N19:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +756,7 @@
       </c>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="12"/>
       <c r="D14" s="12">
         <v>2045</v>
@@ -766,6 +781,28 @@
         <v>12</v>
       </c>
       <c r="N14" s="12"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="12">
+        <v>2046</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1000</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
force to model to build DAC
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC140493-8719-4AA5-A73B-0AE20B3472D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34D94E1-483A-4967-A10B-3E1971350483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>SUPELCAMM01</t>
+  </si>
+  <si>
+    <t>SUPDACELC5N</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="C2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19:N20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +787,7 @@
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D15" s="12">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>15</v>
@@ -806,16 +809,28 @@
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="D16" s="12">
+        <v>2045</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1000</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="M16" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="N16" s="9"/>
     </row>
     <row r="17" spans="10:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
delete activity boundary, but it worked - it was included to check whether the ammonia production works
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579C0AFD-2868-4816-B31C-3A25DC6982C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9CA64-030D-466D-83F6-DA9C5278F7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>ACT_BND</t>
-  </si>
-  <si>
-    <t>SUPELCAMM01</t>
   </si>
 </sst>
 </file>
@@ -565,7 +562,7 @@
   <dimension ref="C2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,26 +780,14 @@
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="12">
-        <v>2045</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12">
-        <v>10</v>
-      </c>
-      <c r="J15" s="12">
-        <v>10</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
input h2 production boundary before 2030 to avoid pre-production
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9CA64-030D-466D-83F6-DA9C5278F7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A356B90-A6F0-4A17-B4B9-2C6A228171E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8976" yWindow="4044" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>ACT_BND</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>DELH2GC</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -272,6 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
@@ -562,19 +569,19 @@
   <dimension ref="C2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -585,7 +592,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -597,7 +604,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -609,7 +616,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -621,7 +628,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
@@ -637,7 +644,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
@@ -675,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C11" s="12"/>
       <c r="D11" s="12">
         <v>2030</v>
@@ -701,7 +708,7 @@
       </c>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C12" s="12"/>
       <c r="D12" s="12">
         <v>2030</v>
@@ -727,7 +734,7 @@
       </c>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C13" s="12"/>
       <c r="D13" s="12">
         <v>2045</v>
@@ -753,7 +760,7 @@
       </c>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="12"/>
       <c r="D14" s="12">
         <v>2045</v>
@@ -779,31 +786,89 @@
       </c>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+    <row r="15" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="I15" s="15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="15">
+        <v>0</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="10:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D17" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>0</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -817,7 +882,7 @@
       <c r="AD17" s="9"/>
       <c r="AE17" s="9"/>
     </row>
-    <row r="18" spans="10:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -859,7 +924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="10:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:31" x14ac:dyDescent="0.3">
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -877,7 +942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="10:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:31" x14ac:dyDescent="0.3">
       <c r="U20">
         <v>2030</v>
       </c>

</xml_diff>

<commit_message>
SUPCO2 Transport boundary added
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A356B90-A6F0-4A17-B4B9-2C6A228171E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8976" yWindow="4044" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19644" yWindow="2364" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>DELH2GC</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISLBH_DKE_02</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +188,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -566,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AE20"/>
+  <dimension ref="C2:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,10 +895,30 @@
       <c r="AE17" s="9"/>
     </row>
     <row r="18" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="12"/>
+      <c r="D18" s="15">
+        <v>2010</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="T18" s="10" t="s">
         <v>8</v>
       </c>
@@ -925,10 +957,31 @@
       </c>
     </row>
     <row r="19" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
+      <c r="D19" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12" t="str">
+        <f>M18</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      </c>
       <c r="U19">
         <v>2030</v>
       </c>
@@ -943,6 +996,31 @@
       </c>
     </row>
     <row r="20" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D20" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0</v>
+      </c>
+      <c r="J20" s="15">
+        <v>0</v>
+      </c>
+      <c r="K20" s="15">
+        <v>0</v>
+      </c>
+      <c r="L20" s="15">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12" t="str">
+        <f t="shared" ref="M20:M21" si="0">M19</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      </c>
       <c r="U20">
         <v>2030</v>
       </c>
@@ -956,7 +1034,142 @@
         <v>18</v>
       </c>
     </row>
+    <row r="21" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D21" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="15">
+        <v>0</v>
+      </c>
+      <c r="K21" s="15">
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="22" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D22" s="15">
+        <v>2010</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="15">
+        <v>0</v>
+      </c>
+      <c r="K22" s="15">
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
+        <v>0</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D23" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12" t="str">
+        <f>M22</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="24" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D24" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15">
+        <v>0</v>
+      </c>
+      <c r="K24" s="15">
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12" t="str">
+        <f t="shared" ref="M24:M25" si="1">M23</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="25" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D25" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="15">
+        <v>0</v>
+      </c>
+      <c r="K25" s="15">
+        <v>0</v>
+      </c>
+      <c r="L25" s="15">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exclude PV & H2 Transport before 2030 in MAR
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF3E27C-091A-452E-B430-596680D1931C}"/>
   <bookViews>
-    <workbookView xWindow="19644" yWindow="2364" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51855" yWindow="3150" windowWidth="20760" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>TB_SUPCO2_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ERSOLPV5N</t>
+  </si>
+  <si>
+    <t>TB_H2_MAR_DKW_01</t>
   </si>
 </sst>
 </file>
@@ -260,7 +269,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -291,15 +300,16 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
     <cellStyle name="Neutral 3" xfId="3" xr:uid="{5B3B309E-6B7E-4D77-AD41-EB17FF9CE808}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{A93E1CA5-B318-4E00-82A5-334EC04E563E}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{C11532E7-AD97-42AD-83FD-AF150A506CCF}"/>
     <cellStyle name="Normal 42" xfId="7" xr:uid="{5C9F8D4D-0E13-4029-9DD1-AB51B39E1F9C}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="1" xr:uid="{5884504C-975A-4531-8909-E98FC51AE458}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="4" xr:uid="{8D4A26F5-E00A-421E-B82B-A50A6798403B}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,22 +588,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AE25"/>
+  <dimension ref="C2:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -603,8 +613,9 @@
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -615,8 +626,9 @@
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M3" s="4"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -627,8 +639,9 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -639,8 +652,9 @@
       <c r="J8" s="1"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
@@ -655,8 +669,9 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
@@ -687,14 +702,17 @@
       <c r="L10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="10" t="s">
-        <v>0</v>
+      <c r="M10" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="N10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C11" s="12"/>
       <c r="D11" s="12">
         <v>2030</v>
@@ -715,12 +733,13 @@
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="12" t="s">
+      <c r="M11" s="13"/>
+      <c r="N11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C12" s="12"/>
       <c r="D12" s="12">
         <v>2030</v>
@@ -741,12 +760,13 @@
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="13"/>
+      <c r="N12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C13" s="12"/>
       <c r="D13" s="12">
         <v>2045</v>
@@ -767,12 +787,13 @@
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="12" t="s">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C14" s="12"/>
       <c r="D14" s="12">
         <v>2045</v>
@@ -793,12 +814,13 @@
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D15" s="15">
         <v>2015</v>
       </c>
@@ -822,11 +844,14 @@
       <c r="L15" s="15">
         <v>0</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C16" s="8"/>
       <c r="D16" s="15">
         <v>2020</v>
@@ -851,12 +876,15 @@
       <c r="L16" s="15">
         <v>0</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+      <c r="N16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D17" s="15">
         <v>2025</v>
       </c>
@@ -878,13 +906,15 @@
       <c r="L17" s="15">
         <v>0</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="15">
+        <v>0</v>
+      </c>
+      <c r="N17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
-      <c r="W17" s="9"/>
+      <c r="W17" s="8"/>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
@@ -893,8 +923,9 @@
       <c r="AC17" s="9"/>
       <c r="AD17" s="9"/>
       <c r="AE17" s="9"/>
-    </row>
-    <row r="18" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF17" s="9"/>
+    </row>
+    <row r="18" spans="4:32" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D18" s="15">
         <v>2010</v>
       </c>
@@ -916,47 +947,50 @@
       <c r="L18" s="15">
         <v>0</v>
       </c>
-      <c r="M18" s="12" t="s">
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="U18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="10" t="s">
+      <c r="V18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="V18" s="10" t="s">
+      <c r="W18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="W18" s="10" t="s">
+      <c r="X18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="X18" s="11" t="s">
+      <c r="Y18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y18" s="11" t="s">
+      <c r="Z18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="Z18" s="11" t="s">
+      <c r="AA18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AA18" s="11" t="s">
+      <c r="AB18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AB18" s="11" t="s">
+      <c r="AC18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AC18" s="11" t="s">
+      <c r="AD18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AD18" s="10" t="s">
-        <v>0</v>
-      </c>
       <c r="AE18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D19" s="15">
         <v>2015</v>
       </c>
@@ -978,24 +1012,27 @@
       <c r="L19" s="15">
         <v>0</v>
       </c>
-      <c r="M19" s="12" t="str">
-        <f>M18</f>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+      <c r="N19" s="12" t="str">
+        <f>N18</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>2030</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>15</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>19</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D20" s="15">
         <v>2020</v>
       </c>
@@ -1017,24 +1054,27 @@
       <c r="L20" s="15">
         <v>0</v>
       </c>
-      <c r="M20" s="12" t="str">
-        <f t="shared" ref="M20:M21" si="0">M19</f>
+      <c r="M20" s="15">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12" t="str">
+        <f t="shared" ref="N20:N21" si="0">N19</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>2030</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>15</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>19</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D21" s="15">
         <v>2025</v>
       </c>
@@ -1056,12 +1096,15 @@
       <c r="L21" s="15">
         <v>0</v>
       </c>
-      <c r="M21" s="12" t="str">
+      <c r="M21" s="15">
+        <v>0</v>
+      </c>
+      <c r="N21" s="12" t="str">
         <f t="shared" si="0"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="22" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D22" s="15">
         <v>2010</v>
       </c>
@@ -1083,11 +1126,14 @@
       <c r="L22" s="15">
         <v>0</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="M22" s="15">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D23" s="15">
         <v>2015</v>
       </c>
@@ -1109,12 +1155,15 @@
       <c r="L23" s="15">
         <v>0</v>
       </c>
-      <c r="M23" s="12" t="str">
-        <f>M22</f>
+      <c r="M23" s="15">
+        <v>0</v>
+      </c>
+      <c r="N23" s="12" t="str">
+        <f>N22</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="24" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D24" s="15">
         <v>2020</v>
       </c>
@@ -1136,12 +1185,15 @@
       <c r="L24" s="15">
         <v>0</v>
       </c>
-      <c r="M24" s="12" t="str">
-        <f t="shared" ref="M24:M25" si="1">M23</f>
+      <c r="M24" s="15">
+        <v>0</v>
+      </c>
+      <c r="N24" s="12" t="str">
+        <f t="shared" ref="N24:N25" si="1">N23</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="25" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D25" s="15">
         <v>2025</v>
       </c>
@@ -1163,9 +1215,190 @@
       <c r="L25" s="15">
         <v>0</v>
       </c>
-      <c r="M25" s="12" t="str">
+      <c r="M25" s="15">
+        <v>0</v>
+      </c>
+      <c r="N25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="26" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D26" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="15">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
+        <v>0</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D27" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="15">
+        <v>0</v>
+      </c>
+      <c r="K27" s="15">
+        <v>0</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0</v>
+      </c>
+      <c r="N27" t="str">
+        <f>N26</f>
+        <v>ERSOLPV5N</v>
+      </c>
+    </row>
+    <row r="28" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D28" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
+        <v>0</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0</v>
+      </c>
+      <c r="N28" t="str">
+        <f>N27</f>
+        <v>ERSOLPV5N</v>
+      </c>
+    </row>
+    <row r="29" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D29" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0</v>
+      </c>
+      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
+        <v>0</v>
+      </c>
+      <c r="M29" s="15">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D30" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
+        <v>0</v>
+      </c>
+      <c r="M30" s="15">
+        <v>0</v>
+      </c>
+      <c r="N30" t="str">
+        <f>N29</f>
+        <v>TB_H2_MAR_DKW_01</v>
+      </c>
+    </row>
+    <row r="31" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D31" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15">
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
+        <v>0</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0</v>
+      </c>
+      <c r="N31" t="str">
+        <f>N30</f>
+        <v>TB_H2_MAR_DKW_01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to put a lower bound on PV in MAR
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF3E27C-091A-452E-B430-596680D1931C}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BACC097A-AFCD-4784-B677-04B3BDB88EDB}"/>
   <bookViews>
-    <workbookView xWindow="51855" yWindow="3150" windowWidth="20760" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47820" yWindow="2820" windowWidth="20760" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>TB_H2_MAR_DKW_01</t>
+  </si>
+  <si>
+    <t>FLO_BND</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AF31"/>
+  <dimension ref="C2:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1401,6 +1404,140 @@
         <v>TB_H2_MAR_DKW_01</v>
       </c>
     </row>
+    <row r="32" spans="4:32" x14ac:dyDescent="0.45">
+      <c r="D32" s="15">
+        <v>0</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="15">
+        <v>4</v>
+      </c>
+      <c r="J32" s="15">
+        <v>4</v>
+      </c>
+      <c r="K32" s="15">
+        <v>4</v>
+      </c>
+      <c r="L32" s="15">
+        <v>4</v>
+      </c>
+      <c r="M32" s="15">
+        <v>4</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D33" s="15">
+        <v>0</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="15">
+        <v>4</v>
+      </c>
+      <c r="J33" s="15">
+        <v>4</v>
+      </c>
+      <c r="K33" s="15">
+        <v>4</v>
+      </c>
+      <c r="L33" s="15">
+        <v>4</v>
+      </c>
+      <c r="M33" s="15">
+        <v>4</v>
+      </c>
+      <c r="N33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D34" s="15">
+        <v>0</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="15">
+        <v>4</v>
+      </c>
+      <c r="J34" s="15">
+        <v>4</v>
+      </c>
+      <c r="K34" s="15">
+        <v>4</v>
+      </c>
+      <c r="L34" s="15">
+        <v>4</v>
+      </c>
+      <c r="M34" s="15">
+        <v>4</v>
+      </c>
+      <c r="N34" t="str">
+        <f>N33</f>
+        <v>TB_H2_MAR_DKW_01</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D35" s="15">
+        <v>0</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="15">
+        <v>4</v>
+      </c>
+      <c r="J35" s="15">
+        <v>4</v>
+      </c>
+      <c r="K35" s="15">
+        <v>4</v>
+      </c>
+      <c r="L35" s="15">
+        <v>4</v>
+      </c>
+      <c r="M35" s="15">
+        <v>4</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D36" s="15">
+        <v>2030</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" s="15">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
input cap boundary for PV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BACC097A-AFCD-4784-B677-04B3BDB88EDB}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ECCFFA9-EF02-4093-AD8A-B1EC18115306}"/>
   <bookViews>
-    <workbookView xWindow="47820" yWindow="2820" windowWidth="20760" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47145" yWindow="2145" windowWidth="20760" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="28">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -591,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AF36"/>
+  <dimension ref="C2:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1538,6 +1538,24 @@
         <v>26</v>
       </c>
     </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D37" s="15">
+        <v>2030</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M37" s="15">
+        <v>1000</v>
+      </c>
+      <c r="N37" t="str">
+        <f>N36</f>
+        <v>TB_H2_MAR_DKW_01</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
boundaries regarding PV in MAR
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD9B5EA-69A0-4FF8-BC03-CC116EB39DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE3DC3-AEA1-4627-8662-B7A8BA87E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="29">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>FLO_BND</t>
+  </si>
+  <si>
+    <t>H2</t>
   </si>
 </sst>
 </file>
@@ -593,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1433,7 +1436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D33" s="15">
         <v>0</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D34" s="15">
         <v>0</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>TB_H2_MAR_DKW_01</v>
       </c>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D35" s="15">
         <v>0</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D36" s="15">
         <v>2030</v>
       </c>
@@ -1537,8 +1540,11 @@
       <c r="N36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="O36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D37" s="15">
         <v>2030</v>
       </c>

</xml_diff>

<commit_message>
update bound on H2 trade
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE3DC3-AEA1-4627-8662-B7A8BA87E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A265B93-1658-496D-8EB3-745F3B4FBED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="4050" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -117,10 +117,10 @@
     <t>TB_H2_MAR_DKW_01</t>
   </si>
   <si>
-    <t>FLO_BND</t>
-  </si>
-  <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>COM_BNDPRD</t>
   </si>
 </sst>
 </file>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1532,7 +1532,7 @@
         <v>15</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M36" s="15">
         <v>1</v>
@@ -1541,7 +1541,7 @@
         <v>26</v>
       </c>
       <c r="O36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update of boundaries to avoid production before 2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsBound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B471775-F024-49F2-A554-B8A63AB6120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F986467B-825C-4E36-A99E-1C576E403205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19644" yWindow="2364" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9708" yWindow="852" windowWidth="20100" windowHeight="15888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="24">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AE25"/>
+  <dimension ref="C2:AE37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,6 +1168,336 @@
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
+    <row r="26" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D26" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="15">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D27" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="15">
+        <v>0</v>
+      </c>
+      <c r="K27" s="15">
+        <v>0</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D28" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
+        <v>0</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D29" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0</v>
+      </c>
+      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
+        <v>0</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D30" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
+        <v>0</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D31" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15">
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
+        <v>0</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D32" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15">
+        <v>0</v>
+      </c>
+      <c r="J32" s="15">
+        <v>0</v>
+      </c>
+      <c r="K32" s="15">
+        <v>0</v>
+      </c>
+      <c r="L32" s="15">
+        <v>0</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D33" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="15">
+        <v>0</v>
+      </c>
+      <c r="J33" s="15">
+        <v>0</v>
+      </c>
+      <c r="K33" s="15">
+        <v>0</v>
+      </c>
+      <c r="L33" s="15">
+        <v>0</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D34" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="15">
+        <v>0</v>
+      </c>
+      <c r="J34" s="15">
+        <v>0</v>
+      </c>
+      <c r="K34" s="15">
+        <v>0</v>
+      </c>
+      <c r="L34" s="15">
+        <v>0</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D35" s="15">
+        <v>2015</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0</v>
+      </c>
+      <c r="J35" s="15">
+        <v>0</v>
+      </c>
+      <c r="K35" s="15">
+        <v>0</v>
+      </c>
+      <c r="L35" s="15">
+        <v>0</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D36" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="15">
+        <v>0</v>
+      </c>
+      <c r="J36" s="15">
+        <v>0</v>
+      </c>
+      <c r="K36" s="15">
+        <v>0</v>
+      </c>
+      <c r="L36" s="15">
+        <v>0</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D37" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="15">
+        <v>0</v>
+      </c>
+      <c r="J37" s="15">
+        <v>0</v>
+      </c>
+      <c r="K37" s="15">
+        <v>0</v>
+      </c>
+      <c r="L37" s="15">
+        <v>0</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>